<commit_message>
Created code to vendor related things
</commit_message>
<xml_diff>
--- a/CustomrePortalPandeyJiDiscussion22may2022.xlsx
+++ b/CustomrePortalPandeyJiDiscussion22may2022.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="80" windowWidth="19140" windowHeight="7340" activeTab="2"/>
+    <workbookView xWindow="75" yWindow="75" windowWidth="19140" windowHeight="7335" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>Admin Screen</t>
   </si>
@@ -234,9 +234,6 @@
     <t xml:space="preserve">Tax Code </t>
   </si>
   <si>
-    <t>Payment Terms</t>
-  </si>
-  <si>
     <t>MasterTable</t>
   </si>
   <si>
@@ -253,6 +250,21 @@
   </si>
   <si>
     <t>Document attached basis on flag yes/no in front of input field</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Nextapprover</t>
+  </si>
+  <si>
+    <t>HOD</t>
+  </si>
+  <si>
+    <t>Legel</t>
+  </si>
+  <si>
+    <t>Last Approver</t>
   </si>
 </sst>
 </file>
@@ -867,9 +879,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="46.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -908,7 +920,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -932,10 +944,10 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="51.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -1042,14 +1054,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="29">
+    <row r="19" spans="2:13" ht="30">
       <c r="E19" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="2:13">
       <c r="E20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -1057,7 +1069,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:13" ht="43.5">
+    <row r="24" spans="2:13" ht="45">
       <c r="E24" s="3" t="s">
         <v>18</v>
       </c>
@@ -1072,7 +1084,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="28">
+    <row r="27" spans="2:13" ht="28.5">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1100,10 +1112,10 @@
     </row>
     <row r="32" spans="2:13">
       <c r="E32" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="4:5" ht="43.5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" ht="45">
       <c r="D35">
         <v>4</v>
       </c>
@@ -1130,11 +1142,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
@@ -1159,19 +1171,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="47.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="19.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="8"/>
@@ -1216,7 +1222,7 @@
       <c r="A5" s="11"/>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:7" ht="14.5" customHeight="1">
+    <row r="6" spans="1:7" ht="14.45" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>35</v>
       </c>
@@ -1287,6 +1293,11 @@
       </c>
       <c r="E13" s="33"/>
       <c r="G13" s="12"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="E15">
+        <v>5322001001</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1307,21 +1318,21 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.7265625" style="21"/>
+    <col min="1" max="1" width="18.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.7109375" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1">
       <c r="A1" s="21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1">
+    <row r="2" spans="1:4" ht="16.5" thickBot="1">
       <c r="A2" s="22" t="s">
         <v>54</v>
       </c>
@@ -1335,7 +1346,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" thickBot="1">
+    <row r="3" spans="1:4" ht="16.5" thickBot="1">
       <c r="A3" s="24" t="s">
         <v>50</v>
       </c>
@@ -1349,7 +1360,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" thickBot="1">
+    <row r="4" spans="1:4" ht="16.5" thickBot="1">
       <c r="A4" s="24" t="s">
         <v>52</v>
       </c>
@@ -1361,7 +1372,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" thickBot="1">
+    <row r="5" spans="1:4" ht="16.5" thickBot="1">
       <c r="A5" s="24" t="s">
         <v>53</v>
       </c>
@@ -1385,25 +1396,25 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="18" t="s">
         <v>57</v>
       </c>
@@ -1411,16 +1422,16 @@
         <v>20</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="18" t="s">
         <v>59</v>
       </c>
@@ -1434,7 +1445,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
@@ -1442,13 +1453,13 @@
         <v>21</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" s="18" t="s">
         <v>62</v>
       </c>
@@ -1462,10 +1473,10 @@
         <v>64</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="18" t="s">
         <v>65</v>
       </c>
@@ -1478,11 +1489,9 @@
       <c r="D6" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="18" t="s">
         <v>67</v>
       </c>
@@ -1490,16 +1499,16 @@
         <v>20</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>60</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="18" t="s">
         <v>68</v>
       </c>
@@ -1512,11 +1521,9 @@
       <c r="D8" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="18" t="s">
         <v>70</v>
       </c>
@@ -1524,30 +1531,51 @@
         <v>20</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>58</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>73</v>
+      <c r="G16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17">
+        <v>10001</v>
+      </c>
+      <c r="C17" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>